<commit_message>
updated Data Description Sheet to match what we actually submitted (pubmed column)
</commit_message>
<xml_diff>
--- a/Data Description Sheet.xlsx
+++ b/Data Description Sheet.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="45">
   <si>
     <t xml:space="preserve">Data Description Sheet</t>
   </si>
@@ -66,6 +66,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">meaningless key, per Species, assigned by </t>
     </r>
@@ -75,6 +76,7 @@
         <color rgb="FF0000FF"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">SNAP</t>
     </r>
@@ -103,6 +105,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">standard Species Name, per the </t>
     </r>
@@ -112,6 +115,7 @@
         <color rgb="FF0000FF"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">NCBI</t>
     </r>
@@ -128,6 +132,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">as in biological taxonomy: Life &gt; </t>
     </r>
@@ -137,6 +142,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Domain</t>
     </r>
@@ -145,6 +151,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> &gt; Kingdom &gt; Phylum ...</t>
     </r>
@@ -175,6 +182,36 @@
   </si>
   <si>
     <t xml:space="preserve">[0, 16887538]</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">the number of </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">PubMed</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> articles about this Species</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Gene Names</t>
@@ -222,6 +259,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -243,18 +281,21 @@
       <sz val="16"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -414,15 +455,15 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C21" activeCellId="0" sqref="C21"/>
+      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="38.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="39.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="54.78"/>
   </cols>
   <sheetData>
@@ -584,54 +625,56 @@
       <c r="D10" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E10" s="6"/>
+      <c r="E10" s="6" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D11" s="7" t="s">
         <v>9</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="8" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D12" s="9" t="s">
         <v>9</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="11" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B14" s="11"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="8" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -642,7 +685,8 @@
   <hyperlinks>
     <hyperlink ref="E4" r:id="rId1" display="SNAP"/>
     <hyperlink ref="E6" r:id="rId2" display="NCBI"/>
-    <hyperlink ref="B15" r:id="rId3" display="https://snap.stanford.edu/tree-of-life/data.html"/>
+    <hyperlink ref="E10" r:id="rId3" display="PubMed"/>
+    <hyperlink ref="B15" r:id="rId4" display="https://snap.stanford.edu/tree-of-life/data.html"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>